<commit_message>
feat: add related function element fix: unable to read format value when exporting bom, unable to restart observable when operation failed
</commit_message>
<xml_diff>
--- a/PID.VisioAddIn/Resources/BOM_template.xlsx
+++ b/PID.VisioAddIn/Resources/BOM_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pid-visio-addin\PID.VisioAddIn\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B3D60C-FEAC-441D-B4B8-7382CC4EB8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD474077-5AD0-4377-83A4-B643A59441F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1680" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="零件清单 Part List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>物料清单 Part List</t>
   </si>
@@ -148,47 +148,87 @@
     <t>Atachment</t>
   </si>
   <si>
-    <t>{{parts.functionalgroup}}</t>
+    <t>{{Parts.ProcessArea}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.name}}</t>
+    <t>{{Parts.FunctionalGroup}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.processarea}}</t>
+    <t>{{Parts.FunctionalElement}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.functionalelement}}</t>
+    <t>{{Parts.AEMaterialNo}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.technicaldata}}</t>
+    <t>{{Parts.NameChinese}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.ingroup}}</t>
+    <t>{{Parts.NameEnglish}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{parts.total}}</t>
+    <t>{{Parts.TechnicalDataChinese}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{customer}}</t>
+    <t>{{Parts.TechnicalDataEnglish}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{project}}</t>
+    <t>{{Parts.Total}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{document}}</t>
+    <t>{{Parts.InGroup}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
-    <t>{{version}}</t>
+    <t>{{Parts.Units}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Attachment}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Classification}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.SerialNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.ManufacturerArticleNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Manufacturer}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Index}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{CustomerName}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{ProjectNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DocumentNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{VersionNo}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -196,7 +236,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,13 +327,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="6">
@@ -471,7 +504,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -574,9 +607,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -597,7 +627,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1132,28 +1162,28 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="14.625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="17.625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21.25" style="7" customWidth="1"/>
-    <col min="9" max="9" width="19.25" style="7" customWidth="1"/>
-    <col min="10" max="10" width="6.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="6" customWidth="1"/>
-    <col min="12" max="12" width="6.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="6" customWidth="1"/>
-    <col min="14" max="14" width="21.75" style="6" customWidth="1"/>
-    <col min="15" max="15" width="15.375" style="6" customWidth="1"/>
-    <col min="16" max="16" width="12.125" style="8" customWidth="1"/>
-    <col min="17" max="17" width="15.375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="13.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="28.75" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.625" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="1.125" style="9" customWidth="1"/>
     <col min="19" max="19" width="16.375" style="10" customWidth="1"/>
     <col min="20" max="20" width="26.875" style="10" customWidth="1"/>
@@ -1161,25 +1191,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="41"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="40"/>
     </row>
     <row r="2" spans="1:21" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
@@ -1189,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>3</v>
@@ -1198,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1224,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>7</v>
@@ -1233,7 +1263,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1252,23 +1282,23 @@
       <c r="U3" s="29"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="44"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="43"/>
       <c r="R4" s="32"/>
       <c r="S4" s="33"/>
       <c r="T4" s="33"/>
@@ -1387,37 +1417,57 @@
       <c r="U6" s="35"/>
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
+      <c r="A7" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="B7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="22" t="s">
+      <c r="E7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="22"/>
+      <c r="F7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="H7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="23"/>
+        <v>48</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="J7" s="22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>53</v>
+      </c>
       <c r="R7" s="37"/>
     </row>
     <row r="8" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat: structural bom support
</commit_message>
<xml_diff>
--- a/PID.VisioAddIn/Resources/BOM_template.xlsx
+++ b/PID.VisioAddIn/Resources/BOM_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pid-visio-addin\PID.VisioAddIn\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD474077-5AD0-4377-83A4-B643A59441F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE3C816-BBA1-4FD0-BF93-0F69C6FF3616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="零件清单 Part List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>物料清单 Part List</t>
   </si>
@@ -229,6 +229,30 @@
   </si>
   <si>
     <t>{{VersionNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Count}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Description}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -373,32 +397,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
@@ -464,19 +462,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
@@ -498,6 +483,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -530,6 +552,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -539,56 +570,47 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -607,23 +629,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -864,13 +886,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>573405</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>1010285</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>219710</xdr:rowOff>
@@ -1159,59 +1181,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:W61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="28.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="16.375" style="10" customWidth="1"/>
-    <col min="20" max="20" width="26.875" style="10" customWidth="1"/>
-    <col min="21" max="16384" width="10" style="10"/>
+    <col min="3" max="3" width="23.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.36328125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="12.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.36328125" style="6" customWidth="1"/>
+    <col min="16" max="16" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="1.08984375" style="9" customWidth="1"/>
+    <col min="21" max="21" width="16.36328125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="26.90625" style="10" customWidth="1"/>
+    <col min="23" max="16384" width="10" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="40"/>
-    </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="43"/>
+    </row>
+    <row r="2" spans="1:23" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1240,13 +1266,14 @@
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="30"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="28"/>
       <c r="T2" s="30"/>
-      <c r="U2" s="29"/>
-    </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U2" s="30"/>
+      <c r="V2" s="29"/>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1275,36 +1302,39 @@
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="30"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="31"/>
       <c r="T3" s="30"/>
-      <c r="U3" s="29"/>
-    </row>
-    <row r="4" spans="1:21" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
-    </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U3" s="30"/>
+      <c r="V3" s="29"/>
+    </row>
+    <row r="4" spans="1:23" s="3" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="34"/>
+    </row>
+    <row r="5" spans="1:23" s="4" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
@@ -1321,47 +1351,53 @@
         <v>13</v>
       </c>
       <c r="F5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="K5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="L5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="M5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="26" t="s">
+      <c r="O5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="P5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="Q5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="R5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
       <c r="T5" s="35"/>
-      <c r="U5" s="36"/>
-    </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="36"/>
+    </row>
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>26</v>
@@ -1376,47 +1412,53 @@
         <v>29</v>
       </c>
       <c r="F6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="J6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="K6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="L6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="M6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="O6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="P6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="Q6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="R6" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="S6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="35"/>
-    </row>
-    <row r="7" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="V6" s="35"/>
+      <c r="W6" s="35"/>
+    </row>
+    <row r="7" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
         <v>58</v>
       </c>
@@ -1433,44 +1475,50 @@
         <v>45</v>
       </c>
       <c r="F7" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="I7" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="K7" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="L7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="M7" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="O7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="P7" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="Q7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="R7" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" s="22" t="s">
+      <c r="S7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="R7" s="37"/>
-    </row>
-    <row r="8" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="T7" s="37"/>
+    </row>
+    <row r="8" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="22"/>
@@ -1478,19 +1526,21 @@
       <c r="E8" s="24"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="25"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="24"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="27"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="24"/>
-      <c r="R8" s="37"/>
-    </row>
-    <row r="9" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R8" s="27"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="37"/>
+    </row>
+    <row r="9" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="22"/>
@@ -1498,19 +1548,21 @@
       <c r="E9" s="24"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="25"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="25"/>
-      <c r="J9" s="24"/>
+      <c r="J9" s="25"/>
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
-      <c r="P9" s="27"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="24"/>
-      <c r="R9" s="37"/>
-    </row>
-    <row r="10" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R9" s="27"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="37"/>
+    </row>
+    <row r="10" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="22"/>
@@ -1518,19 +1570,21 @@
       <c r="E10" s="24"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="25"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="25"/>
-      <c r="J10" s="24"/>
+      <c r="J10" s="25"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
       <c r="O10" s="24"/>
-      <c r="P10" s="27"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
-      <c r="R10" s="37"/>
-    </row>
-    <row r="11" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R10" s="27"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="37"/>
+    </row>
+    <row r="11" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="22"/>
@@ -1538,19 +1592,21 @@
       <c r="E11" s="24"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="25"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="25"/>
-      <c r="J11" s="24"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
-      <c r="P11" s="27"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
-      <c r="R11" s="37"/>
-    </row>
-    <row r="12" spans="1:21" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R11" s="27"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="37"/>
+    </row>
+    <row r="12" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="22"/>
@@ -1558,19 +1614,21 @@
       <c r="E12" s="24"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="25"/>
-      <c r="J12" s="24"/>
+      <c r="J12" s="25"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
-      <c r="P12" s="27"/>
+      <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
-      <c r="R12" s="37"/>
-    </row>
-    <row r="13" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R12" s="27"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="37"/>
+    </row>
+    <row r="13" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="22"/>
@@ -1578,18 +1636,20 @@
       <c r="E13" s="24"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="25"/>
-      <c r="J13" s="24"/>
+      <c r="J13" s="25"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
-      <c r="P13" s="27"/>
+      <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
-    </row>
-    <row r="14" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R13" s="27"/>
+      <c r="S13" s="24"/>
+    </row>
+    <row r="14" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="22"/>
@@ -1597,18 +1657,20 @@
       <c r="E14" s="24"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="25"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="24"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
-      <c r="P14" s="27"/>
+      <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
-    </row>
-    <row r="15" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R14" s="27"/>
+      <c r="S14" s="24"/>
+    </row>
+    <row r="15" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="22"/>
@@ -1616,18 +1678,20 @@
       <c r="E15" s="24"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="25"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="25"/>
-      <c r="J15" s="24"/>
+      <c r="J15" s="25"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="27"/>
+      <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-    </row>
-    <row r="16" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R15" s="27"/>
+      <c r="S15" s="24"/>
+    </row>
+    <row r="16" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="22"/>
@@ -1635,18 +1699,20 @@
       <c r="E16" s="24"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="25"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="25"/>
-      <c r="J16" s="24"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
-      <c r="P16" s="27"/>
+      <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
-    </row>
-    <row r="17" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R16" s="27"/>
+      <c r="S16" s="24"/>
+    </row>
+    <row r="17" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="22"/>
@@ -1654,18 +1720,20 @@
       <c r="E17" s="24"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="25"/>
+      <c r="H17" s="22"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="24"/>
+      <c r="J17" s="25"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
-      <c r="P17" s="27"/>
+      <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
-    </row>
-    <row r="18" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R17" s="27"/>
+      <c r="S17" s="24"/>
+    </row>
+    <row r="18" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="22"/>
@@ -1673,18 +1741,20 @@
       <c r="E18" s="24"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="25"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="24"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
-      <c r="P18" s="27"/>
+      <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
-    </row>
-    <row r="19" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R18" s="27"/>
+      <c r="S18" s="24"/>
+    </row>
+    <row r="19" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="22"/>
@@ -1692,18 +1762,20 @@
       <c r="E19" s="24"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="25"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="24"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="27"/>
+      <c r="P19" s="24"/>
       <c r="Q19" s="24"/>
-    </row>
-    <row r="20" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R19" s="27"/>
+      <c r="S19" s="24"/>
+    </row>
+    <row r="20" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="22"/>
@@ -1711,18 +1783,20 @@
       <c r="E20" s="24"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="25"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="24"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
-      <c r="P20" s="27"/>
+      <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
-    </row>
-    <row r="21" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R20" s="27"/>
+      <c r="S20" s="24"/>
+    </row>
+    <row r="21" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="22"/>
@@ -1730,18 +1804,20 @@
       <c r="E21" s="24"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="25"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="24"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="27"/>
+      <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
-    </row>
-    <row r="22" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R21" s="27"/>
+      <c r="S21" s="24"/>
+    </row>
+    <row r="22" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="22"/>
@@ -1749,18 +1825,20 @@
       <c r="E22" s="24"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="25"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="25"/>
-      <c r="J22" s="24"/>
+      <c r="J22" s="25"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
-      <c r="P22" s="27"/>
+      <c r="P22" s="24"/>
       <c r="Q22" s="24"/>
-    </row>
-    <row r="23" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R22" s="27"/>
+      <c r="S22" s="24"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="22"/>
@@ -1768,18 +1846,20 @@
       <c r="E23" s="24"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="25"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="25"/>
-      <c r="J23" s="24"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
-      <c r="P23" s="27"/>
+      <c r="P23" s="24"/>
       <c r="Q23" s="24"/>
-    </row>
-    <row r="24" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R23" s="27"/>
+      <c r="S23" s="24"/>
+    </row>
+    <row r="24" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="22"/>
@@ -1787,18 +1867,20 @@
       <c r="E24" s="24"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="25"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="25"/>
-      <c r="J24" s="24"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
-      <c r="P24" s="27"/>
+      <c r="P24" s="24"/>
       <c r="Q24" s="24"/>
-    </row>
-    <row r="25" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R24" s="27"/>
+      <c r="S24" s="24"/>
+    </row>
+    <row r="25" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A25" s="22"/>
       <c r="B25" s="23"/>
       <c r="C25" s="22"/>
@@ -1806,18 +1888,20 @@
       <c r="E25" s="24"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="25"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="25"/>
-      <c r="J25" s="24"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
-      <c r="P25" s="27"/>
+      <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
-    </row>
-    <row r="26" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R25" s="27"/>
+      <c r="S25" s="24"/>
+    </row>
+    <row r="26" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A26" s="22"/>
       <c r="B26" s="23"/>
       <c r="C26" s="22"/>
@@ -1825,18 +1909,20 @@
       <c r="E26" s="24"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="25"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="25"/>
-      <c r="J26" s="24"/>
+      <c r="J26" s="25"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
-      <c r="P26" s="27"/>
+      <c r="P26" s="24"/>
       <c r="Q26" s="24"/>
-    </row>
-    <row r="27" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R26" s="27"/>
+      <c r="S26" s="24"/>
+    </row>
+    <row r="27" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A27" s="22"/>
       <c r="B27" s="23"/>
       <c r="C27" s="22"/>
@@ -1844,18 +1930,20 @@
       <c r="E27" s="24"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="25"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="25"/>
-      <c r="J27" s="24"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
       <c r="O27" s="24"/>
-      <c r="P27" s="27"/>
+      <c r="P27" s="24"/>
       <c r="Q27" s="24"/>
-    </row>
-    <row r="28" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R27" s="27"/>
+      <c r="S27" s="24"/>
+    </row>
+    <row r="28" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="22"/>
@@ -1863,18 +1951,20 @@
       <c r="E28" s="24"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="25"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="25"/>
-      <c r="J28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
       <c r="O28" s="24"/>
-      <c r="P28" s="27"/>
+      <c r="P28" s="24"/>
       <c r="Q28" s="24"/>
-    </row>
-    <row r="29" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R28" s="27"/>
+      <c r="S28" s="24"/>
+    </row>
+    <row r="29" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A29" s="22"/>
       <c r="B29" s="23"/>
       <c r="C29" s="22"/>
@@ -1882,18 +1972,20 @@
       <c r="E29" s="24"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="25"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="25"/>
-      <c r="J29" s="24"/>
+      <c r="J29" s="25"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
       <c r="O29" s="24"/>
-      <c r="P29" s="27"/>
+      <c r="P29" s="24"/>
       <c r="Q29" s="24"/>
-    </row>
-    <row r="30" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R29" s="27"/>
+      <c r="S29" s="24"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A30" s="22"/>
       <c r="B30" s="23"/>
       <c r="C30" s="22"/>
@@ -1901,18 +1993,20 @@
       <c r="E30" s="24"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="25"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="25"/>
-      <c r="J30" s="24"/>
+      <c r="J30" s="25"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="24"/>
-      <c r="P30" s="27"/>
+      <c r="P30" s="24"/>
       <c r="Q30" s="24"/>
-    </row>
-    <row r="31" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R30" s="27"/>
+      <c r="S30" s="24"/>
+    </row>
+    <row r="31" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="22"/>
@@ -1920,18 +2014,20 @@
       <c r="E31" s="24"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="25"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="25"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
-      <c r="P31" s="27"/>
+      <c r="P31" s="24"/>
       <c r="Q31" s="24"/>
-    </row>
-    <row r="32" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R31" s="27"/>
+      <c r="S31" s="24"/>
+    </row>
+    <row r="32" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A32" s="22"/>
       <c r="B32" s="23"/>
       <c r="C32" s="22"/>
@@ -1939,18 +2035,20 @@
       <c r="E32" s="24"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="25"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="25"/>
-      <c r="J32" s="24"/>
+      <c r="J32" s="25"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
       <c r="O32" s="24"/>
-      <c r="P32" s="27"/>
+      <c r="P32" s="24"/>
       <c r="Q32" s="24"/>
-    </row>
-    <row r="33" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R32" s="27"/>
+      <c r="S32" s="24"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="22"/>
@@ -1958,18 +2056,20 @@
       <c r="E33" s="24"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="25"/>
+      <c r="H33" s="22"/>
       <c r="I33" s="25"/>
-      <c r="J33" s="24"/>
+      <c r="J33" s="25"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
       <c r="N33" s="24"/>
       <c r="O33" s="24"/>
-      <c r="P33" s="27"/>
+      <c r="P33" s="24"/>
       <c r="Q33" s="24"/>
-    </row>
-    <row r="34" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R33" s="27"/>
+      <c r="S33" s="24"/>
+    </row>
+    <row r="34" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A34" s="22"/>
       <c r="B34" s="23"/>
       <c r="C34" s="22"/>
@@ -1977,18 +2077,20 @@
       <c r="E34" s="24"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="25"/>
-      <c r="J34" s="24"/>
+      <c r="J34" s="25"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" s="24"/>
       <c r="O34" s="24"/>
-      <c r="P34" s="27"/>
+      <c r="P34" s="24"/>
       <c r="Q34" s="24"/>
-    </row>
-    <row r="35" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R34" s="27"/>
+      <c r="S34" s="24"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A35" s="22"/>
       <c r="B35" s="23"/>
       <c r="C35" s="22"/>
@@ -1996,18 +2098,20 @@
       <c r="E35" s="24"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="25"/>
+      <c r="H35" s="22"/>
       <c r="I35" s="25"/>
-      <c r="J35" s="24"/>
+      <c r="J35" s="25"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" s="24"/>
       <c r="O35" s="24"/>
-      <c r="P35" s="27"/>
+      <c r="P35" s="24"/>
       <c r="Q35" s="24"/>
-    </row>
-    <row r="36" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R35" s="27"/>
+      <c r="S35" s="24"/>
+    </row>
+    <row r="36" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A36" s="22"/>
       <c r="B36" s="23"/>
       <c r="C36" s="22"/>
@@ -2015,18 +2119,20 @@
       <c r="E36" s="24"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="25"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="25"/>
-      <c r="J36" s="24"/>
+      <c r="J36" s="25"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
       <c r="O36" s="24"/>
-      <c r="P36" s="27"/>
+      <c r="P36" s="24"/>
       <c r="Q36" s="24"/>
-    </row>
-    <row r="37" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R36" s="27"/>
+      <c r="S36" s="24"/>
+    </row>
+    <row r="37" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A37" s="22"/>
       <c r="B37" s="23"/>
       <c r="C37" s="22"/>
@@ -2034,18 +2140,20 @@
       <c r="E37" s="24"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="25"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="24"/>
+      <c r="J37" s="25"/>
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
-      <c r="P37" s="27"/>
+      <c r="P37" s="24"/>
       <c r="Q37" s="24"/>
-    </row>
-    <row r="38" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R37" s="27"/>
+      <c r="S37" s="24"/>
+    </row>
+    <row r="38" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A38" s="22"/>
       <c r="B38" s="23"/>
       <c r="C38" s="22"/>
@@ -2053,18 +2161,20 @@
       <c r="E38" s="24"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="25"/>
+      <c r="H38" s="22"/>
       <c r="I38" s="25"/>
-      <c r="J38" s="24"/>
+      <c r="J38" s="25"/>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
       <c r="O38" s="24"/>
-      <c r="P38" s="27"/>
+      <c r="P38" s="24"/>
       <c r="Q38" s="24"/>
-    </row>
-    <row r="39" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R38" s="27"/>
+      <c r="S38" s="24"/>
+    </row>
+    <row r="39" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="22"/>
@@ -2072,18 +2182,20 @@
       <c r="E39" s="24"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="25"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="25"/>
-      <c r="J39" s="24"/>
+      <c r="J39" s="25"/>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
       <c r="O39" s="24"/>
-      <c r="P39" s="27"/>
+      <c r="P39" s="24"/>
       <c r="Q39" s="24"/>
-    </row>
-    <row r="40" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R39" s="27"/>
+      <c r="S39" s="24"/>
+    </row>
+    <row r="40" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A40" s="22"/>
       <c r="B40" s="23"/>
       <c r="C40" s="22"/>
@@ -2091,18 +2203,20 @@
       <c r="E40" s="24"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
-      <c r="H40" s="25"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="25"/>
-      <c r="J40" s="24"/>
+      <c r="J40" s="25"/>
       <c r="K40" s="24"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
       <c r="O40" s="24"/>
-      <c r="P40" s="27"/>
+      <c r="P40" s="24"/>
       <c r="Q40" s="24"/>
-    </row>
-    <row r="41" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R40" s="27"/>
+      <c r="S40" s="24"/>
+    </row>
+    <row r="41" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A41" s="22"/>
       <c r="B41" s="23"/>
       <c r="C41" s="22"/>
@@ -2110,18 +2224,20 @@
       <c r="E41" s="24"/>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="25"/>
-      <c r="J41" s="24"/>
+      <c r="J41" s="25"/>
       <c r="K41" s="24"/>
       <c r="L41" s="24"/>
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
       <c r="O41" s="24"/>
-      <c r="P41" s="27"/>
+      <c r="P41" s="24"/>
       <c r="Q41" s="24"/>
-    </row>
-    <row r="42" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R41" s="27"/>
+      <c r="S41" s="24"/>
+    </row>
+    <row r="42" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A42" s="22"/>
       <c r="B42" s="23"/>
       <c r="C42" s="22"/>
@@ -2129,18 +2245,20 @@
       <c r="E42" s="24"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="25"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="25"/>
-      <c r="J42" s="24"/>
+      <c r="J42" s="25"/>
       <c r="K42" s="24"/>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
       <c r="N42" s="24"/>
       <c r="O42" s="24"/>
-      <c r="P42" s="27"/>
+      <c r="P42" s="24"/>
       <c r="Q42" s="24"/>
-    </row>
-    <row r="43" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R42" s="27"/>
+      <c r="S42" s="24"/>
+    </row>
+    <row r="43" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A43" s="22"/>
       <c r="B43" s="23"/>
       <c r="C43" s="22"/>
@@ -2148,18 +2266,20 @@
       <c r="E43" s="24"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="25"/>
+      <c r="H43" s="22"/>
       <c r="I43" s="25"/>
-      <c r="J43" s="24"/>
+      <c r="J43" s="25"/>
       <c r="K43" s="24"/>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
       <c r="O43" s="24"/>
-      <c r="P43" s="27"/>
+      <c r="P43" s="24"/>
       <c r="Q43" s="24"/>
-    </row>
-    <row r="44" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R43" s="27"/>
+      <c r="S43" s="24"/>
+    </row>
+    <row r="44" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A44" s="22"/>
       <c r="B44" s="23"/>
       <c r="C44" s="22"/>
@@ -2167,18 +2287,20 @@
       <c r="E44" s="24"/>
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
-      <c r="H44" s="25"/>
+      <c r="H44" s="22"/>
       <c r="I44" s="25"/>
-      <c r="J44" s="24"/>
+      <c r="J44" s="25"/>
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
       <c r="N44" s="24"/>
       <c r="O44" s="24"/>
-      <c r="P44" s="27"/>
+      <c r="P44" s="24"/>
       <c r="Q44" s="24"/>
-    </row>
-    <row r="45" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R44" s="27"/>
+      <c r="S44" s="24"/>
+    </row>
+    <row r="45" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A45" s="22"/>
       <c r="B45" s="23"/>
       <c r="C45" s="22"/>
@@ -2186,18 +2308,20 @@
       <c r="E45" s="24"/>
       <c r="F45" s="22"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="25"/>
-      <c r="J45" s="24"/>
+      <c r="J45" s="25"/>
       <c r="K45" s="24"/>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="24"/>
       <c r="O45" s="24"/>
-      <c r="P45" s="27"/>
+      <c r="P45" s="24"/>
       <c r="Q45" s="24"/>
-    </row>
-    <row r="46" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R45" s="27"/>
+      <c r="S45" s="24"/>
+    </row>
+    <row r="46" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A46" s="22"/>
       <c r="B46" s="23"/>
       <c r="C46" s="22"/>
@@ -2205,18 +2329,20 @@
       <c r="E46" s="24"/>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="25"/>
+      <c r="H46" s="22"/>
       <c r="I46" s="25"/>
-      <c r="J46" s="24"/>
+      <c r="J46" s="25"/>
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
       <c r="N46" s="24"/>
       <c r="O46" s="24"/>
-      <c r="P46" s="27"/>
+      <c r="P46" s="24"/>
       <c r="Q46" s="24"/>
-    </row>
-    <row r="47" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R46" s="27"/>
+      <c r="S46" s="24"/>
+    </row>
+    <row r="47" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A47" s="22"/>
       <c r="B47" s="23"/>
       <c r="C47" s="22"/>
@@ -2224,18 +2350,20 @@
       <c r="E47" s="24"/>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
-      <c r="H47" s="25"/>
+      <c r="H47" s="22"/>
       <c r="I47" s="25"/>
-      <c r="J47" s="24"/>
+      <c r="J47" s="25"/>
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
       <c r="N47" s="24"/>
       <c r="O47" s="24"/>
-      <c r="P47" s="27"/>
+      <c r="P47" s="24"/>
       <c r="Q47" s="24"/>
-    </row>
-    <row r="48" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R47" s="27"/>
+      <c r="S47" s="24"/>
+    </row>
+    <row r="48" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A48" s="22"/>
       <c r="B48" s="23"/>
       <c r="C48" s="22"/>
@@ -2243,18 +2371,20 @@
       <c r="E48" s="24"/>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="22"/>
       <c r="I48" s="25"/>
-      <c r="J48" s="24"/>
+      <c r="J48" s="25"/>
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
       <c r="N48" s="24"/>
       <c r="O48" s="24"/>
-      <c r="P48" s="27"/>
+      <c r="P48" s="24"/>
       <c r="Q48" s="24"/>
-    </row>
-    <row r="49" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R48" s="27"/>
+      <c r="S48" s="24"/>
+    </row>
+    <row r="49" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A49" s="22"/>
       <c r="B49" s="23"/>
       <c r="C49" s="22"/>
@@ -2262,18 +2392,20 @@
       <c r="E49" s="24"/>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="22"/>
       <c r="I49" s="25"/>
-      <c r="J49" s="24"/>
+      <c r="J49" s="25"/>
       <c r="K49" s="24"/>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" s="24"/>
       <c r="O49" s="24"/>
-      <c r="P49" s="27"/>
+      <c r="P49" s="24"/>
       <c r="Q49" s="24"/>
-    </row>
-    <row r="50" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R49" s="27"/>
+      <c r="S49" s="24"/>
+    </row>
+    <row r="50" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A50" s="22"/>
       <c r="B50" s="23"/>
       <c r="C50" s="22"/>
@@ -2281,18 +2413,20 @@
       <c r="E50" s="24"/>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
-      <c r="H50" s="25"/>
+      <c r="H50" s="22"/>
       <c r="I50" s="25"/>
-      <c r="J50" s="24"/>
+      <c r="J50" s="25"/>
       <c r="K50" s="24"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
       <c r="O50" s="24"/>
-      <c r="P50" s="27"/>
+      <c r="P50" s="24"/>
       <c r="Q50" s="24"/>
-    </row>
-    <row r="51" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R50" s="27"/>
+      <c r="S50" s="24"/>
+    </row>
+    <row r="51" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A51" s="22"/>
       <c r="B51" s="23"/>
       <c r="C51" s="22"/>
@@ -2300,18 +2434,20 @@
       <c r="E51" s="24"/>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
-      <c r="H51" s="25"/>
+      <c r="H51" s="22"/>
       <c r="I51" s="25"/>
-      <c r="J51" s="24"/>
+      <c r="J51" s="25"/>
       <c r="K51" s="24"/>
       <c r="L51" s="24"/>
       <c r="M51" s="24"/>
       <c r="N51" s="24"/>
       <c r="O51" s="24"/>
-      <c r="P51" s="27"/>
+      <c r="P51" s="24"/>
       <c r="Q51" s="24"/>
-    </row>
-    <row r="52" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R51" s="27"/>
+      <c r="S51" s="24"/>
+    </row>
+    <row r="52" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A52" s="22"/>
       <c r="B52" s="23"/>
       <c r="C52" s="22"/>
@@ -2319,18 +2455,20 @@
       <c r="E52" s="24"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
-      <c r="H52" s="25"/>
+      <c r="H52" s="22"/>
       <c r="I52" s="25"/>
-      <c r="J52" s="24"/>
+      <c r="J52" s="25"/>
       <c r="K52" s="24"/>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
       <c r="N52" s="24"/>
       <c r="O52" s="24"/>
-      <c r="P52" s="27"/>
+      <c r="P52" s="24"/>
       <c r="Q52" s="24"/>
-    </row>
-    <row r="53" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R52" s="27"/>
+      <c r="S52" s="24"/>
+    </row>
+    <row r="53" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A53" s="22"/>
       <c r="B53" s="23"/>
       <c r="C53" s="22"/>
@@ -2338,18 +2476,20 @@
       <c r="E53" s="24"/>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="25"/>
+      <c r="H53" s="22"/>
       <c r="I53" s="25"/>
-      <c r="J53" s="24"/>
+      <c r="J53" s="25"/>
       <c r="K53" s="24"/>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
       <c r="N53" s="24"/>
       <c r="O53" s="24"/>
-      <c r="P53" s="27"/>
+      <c r="P53" s="24"/>
       <c r="Q53" s="24"/>
-    </row>
-    <row r="54" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R53" s="27"/>
+      <c r="S53" s="24"/>
+    </row>
+    <row r="54" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A54" s="22"/>
       <c r="B54" s="23"/>
       <c r="C54" s="22"/>
@@ -2357,18 +2497,20 @@
       <c r="E54" s="24"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
-      <c r="H54" s="25"/>
+      <c r="H54" s="22"/>
       <c r="I54" s="25"/>
-      <c r="J54" s="24"/>
+      <c r="J54" s="25"/>
       <c r="K54" s="24"/>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
       <c r="N54" s="24"/>
       <c r="O54" s="24"/>
-      <c r="P54" s="27"/>
+      <c r="P54" s="24"/>
       <c r="Q54" s="24"/>
-    </row>
-    <row r="55" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R54" s="27"/>
+      <c r="S54" s="24"/>
+    </row>
+    <row r="55" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A55" s="22"/>
       <c r="B55" s="23"/>
       <c r="C55" s="22"/>
@@ -2376,18 +2518,20 @@
       <c r="E55" s="24"/>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
-      <c r="H55" s="25"/>
+      <c r="H55" s="22"/>
       <c r="I55" s="25"/>
-      <c r="J55" s="24"/>
+      <c r="J55" s="25"/>
       <c r="K55" s="24"/>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
       <c r="N55" s="24"/>
       <c r="O55" s="24"/>
-      <c r="P55" s="27"/>
+      <c r="P55" s="24"/>
       <c r="Q55" s="24"/>
-    </row>
-    <row r="56" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R55" s="27"/>
+      <c r="S55" s="24"/>
+    </row>
+    <row r="56" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A56" s="22"/>
       <c r="B56" s="23"/>
       <c r="C56" s="22"/>
@@ -2395,18 +2539,20 @@
       <c r="E56" s="24"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
-      <c r="H56" s="25"/>
+      <c r="H56" s="22"/>
       <c r="I56" s="25"/>
-      <c r="J56" s="24"/>
+      <c r="J56" s="25"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
       <c r="M56" s="24"/>
       <c r="N56" s="24"/>
       <c r="O56" s="24"/>
-      <c r="P56" s="27"/>
+      <c r="P56" s="24"/>
       <c r="Q56" s="24"/>
-    </row>
-    <row r="57" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R56" s="27"/>
+      <c r="S56" s="24"/>
+    </row>
+    <row r="57" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A57" s="22"/>
       <c r="B57" s="23"/>
       <c r="C57" s="22"/>
@@ -2414,18 +2560,20 @@
       <c r="E57" s="24"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
-      <c r="H57" s="25"/>
+      <c r="H57" s="22"/>
       <c r="I57" s="25"/>
-      <c r="J57" s="24"/>
+      <c r="J57" s="25"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
       <c r="N57" s="24"/>
       <c r="O57" s="24"/>
-      <c r="P57" s="27"/>
+      <c r="P57" s="24"/>
       <c r="Q57" s="24"/>
-    </row>
-    <row r="58" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R57" s="27"/>
+      <c r="S57" s="24"/>
+    </row>
+    <row r="58" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A58" s="22"/>
       <c r="B58" s="23"/>
       <c r="C58" s="22"/>
@@ -2433,18 +2581,20 @@
       <c r="E58" s="24"/>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
-      <c r="H58" s="25"/>
+      <c r="H58" s="22"/>
       <c r="I58" s="25"/>
-      <c r="J58" s="24"/>
+      <c r="J58" s="25"/>
       <c r="K58" s="24"/>
       <c r="L58" s="24"/>
       <c r="M58" s="24"/>
       <c r="N58" s="24"/>
       <c r="O58" s="24"/>
-      <c r="P58" s="27"/>
+      <c r="P58" s="24"/>
       <c r="Q58" s="24"/>
-    </row>
-    <row r="59" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R58" s="27"/>
+      <c r="S58" s="24"/>
+    </row>
+    <row r="59" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A59" s="22"/>
       <c r="B59" s="23"/>
       <c r="C59" s="22"/>
@@ -2452,18 +2602,20 @@
       <c r="E59" s="24"/>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
-      <c r="H59" s="25"/>
+      <c r="H59" s="22"/>
       <c r="I59" s="25"/>
-      <c r="J59" s="24"/>
+      <c r="J59" s="25"/>
       <c r="K59" s="24"/>
       <c r="L59" s="24"/>
       <c r="M59" s="24"/>
       <c r="N59" s="24"/>
       <c r="O59" s="24"/>
-      <c r="P59" s="27"/>
+      <c r="P59" s="24"/>
       <c r="Q59" s="24"/>
-    </row>
-    <row r="60" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R59" s="27"/>
+      <c r="S59" s="24"/>
+    </row>
+    <row r="60" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A60" s="22"/>
       <c r="B60" s="23"/>
       <c r="C60" s="22"/>
@@ -2471,18 +2623,20 @@
       <c r="E60" s="24"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
-      <c r="H60" s="25"/>
+      <c r="H60" s="22"/>
       <c r="I60" s="25"/>
-      <c r="J60" s="24"/>
+      <c r="J60" s="25"/>
       <c r="K60" s="24"/>
       <c r="L60" s="24"/>
       <c r="M60" s="24"/>
       <c r="N60" s="24"/>
       <c r="O60" s="24"/>
-      <c r="P60" s="27"/>
+      <c r="P60" s="24"/>
       <c r="Q60" s="24"/>
-    </row>
-    <row r="61" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="R60" s="27"/>
+      <c r="S60" s="24"/>
+    </row>
+    <row r="61" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A61" s="22"/>
       <c r="B61" s="23"/>
       <c r="C61" s="22"/>
@@ -2490,21 +2644,23 @@
       <c r="E61" s="24"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="25"/>
+      <c r="H61" s="22"/>
       <c r="I61" s="25"/>
-      <c r="J61" s="24"/>
+      <c r="J61" s="25"/>
       <c r="K61" s="24"/>
       <c r="L61" s="24"/>
       <c r="M61" s="24"/>
       <c r="N61" s="24"/>
       <c r="O61" s="24"/>
-      <c r="P61" s="27"/>
+      <c r="P61" s="24"/>
       <c r="Q61" s="24"/>
+      <c r="R61" s="27"/>
+      <c r="S61" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A4:Q4"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A4:S4"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: export to page
Signed-off-by: Snailya <snailya2005@gmail.com>
</commit_message>
<xml_diff>
--- a/PID.VisioAddIn/Resources/BOM_template.xlsx
+++ b/PID.VisioAddIn/Resources/BOM_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pid-visio-addin\PID.VisioAddIn\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03-程序\AE-PID\PID.VisioAddIn\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE3C816-BBA1-4FD0-BF93-0F69C6FF3616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFD500-5F5C-40A6-898B-5486FF8B1E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="零件清单 Part List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>物料清单 Part List</t>
   </si>
@@ -52,207 +52,210 @@
     <t>序号</t>
   </si>
   <si>
-    <t>工艺区域</t>
-  </si>
-  <si>
     <t>功能组</t>
   </si>
   <si>
     <t>功能元件</t>
   </si>
   <si>
-    <t>AE 物料编码</t>
-  </si>
-  <si>
-    <t>名称-中文</t>
-  </si>
-  <si>
-    <t>名称-英文</t>
+    <t>技术参数-英文</t>
+  </si>
+  <si>
+    <t>组内数量</t>
+  </si>
+  <si>
+    <t>单位</t>
+  </si>
+  <si>
+    <t>型号</t>
+  </si>
+  <si>
+    <t>分类</t>
+  </si>
+  <si>
+    <t>附件</t>
+  </si>
+  <si>
+    <t>Functional Group</t>
+  </si>
+  <si>
+    <t>Function Element</t>
+  </si>
+  <si>
+    <t>Technical data - Chinese</t>
+  </si>
+  <si>
+    <t>Technical data - English</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>In group</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Atachment</t>
+  </si>
+  <si>
+    <t>{{Parts.ProcessArea}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.FunctionalGroup}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.FunctionalElement}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.TechnicalDataChinese}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.TechnicalDataEnglish}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Total}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.InGroup}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Attachment}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Classification}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Index}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{CustomerName}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{ProjectNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{DocumentNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{VersionNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Count}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Description}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域号</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area No.</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>物料号</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Material No.</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>规格</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Specification</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Specification}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.MaterialNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>供应商</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Supplier</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Supplier}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Type}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>技术参数-中文</t>
-  </si>
-  <si>
-    <t>技术参数-英文</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>总数量</t>
-  </si>
-  <si>
-    <t>组内数量</t>
-  </si>
-  <si>
-    <t>单位</t>
-  </si>
-  <si>
-    <t>制造商</t>
-  </si>
-  <si>
-    <t>制造商物品编号</t>
-  </si>
-  <si>
-    <t>型号</t>
-  </si>
-  <si>
-    <t>分类</t>
-  </si>
-  <si>
-    <t>附件</t>
-  </si>
-  <si>
-    <t>Process Area</t>
-  </si>
-  <si>
-    <t>Functional Group</t>
-  </si>
-  <si>
-    <t>Function Element</t>
-  </si>
-  <si>
-    <t>AE Material No.</t>
-  </si>
-  <si>
-    <t>Name - Chinese</t>
-  </si>
-  <si>
-    <t>Name - English</t>
-  </si>
-  <si>
-    <t>Technical data - Chinese</t>
-  </si>
-  <si>
-    <t>Technical data - English</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>In group</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Manufacturer article  No.</t>
-  </si>
-  <si>
-    <t>Serial no.</t>
-  </si>
-  <si>
-    <t>Classification</t>
-  </si>
-  <si>
-    <t>Atachment</t>
-  </si>
-  <si>
-    <t>{{Parts.ProcessArea}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.FunctionalGroup}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.FunctionalElement}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.AEMaterialNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.NameChinese}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.NameEnglish}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.TechnicalDataChinese}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.TechnicalDataEnglish}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Total}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.InGroup}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Units}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Attachment}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Classification}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.SerialNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.ManufacturerArticleNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Manufacturer}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Index}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{CustomerName}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{ProjectNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{DocumentNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{VersionNo}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Count}}</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>{{Parts.Description}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>制造商物料号</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manufacturer Material  No.</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.ManufacturerMaterialNo}}</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>{{Parts.Unit}}</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -629,6 +632,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -637,15 +649,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,13 +889,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>573405</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1010285</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>219710</xdr:rowOff>
@@ -1181,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1196,48 +1199,46 @@
     <col min="5" max="5" width="20.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6328125" style="6" customWidth="1"/>
     <col min="7" max="7" width="20.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.36328125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.36328125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="1.08984375" style="9" customWidth="1"/>
-    <col min="21" max="21" width="16.36328125" style="10" customWidth="1"/>
-    <col min="22" max="22" width="26.90625" style="10" customWidth="1"/>
-    <col min="23" max="16384" width="10" style="10"/>
+    <col min="8" max="8" width="27.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.36328125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.36328125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="28.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.08984375" style="9" customWidth="1"/>
+    <col min="20" max="20" width="16.36328125" style="10" customWidth="1"/>
+    <col min="21" max="21" width="26.90625" style="10" customWidth="1"/>
+    <col min="22" max="16384" width="10" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="43"/>
-    </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>3</v>
@@ -1254,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -1267,13 +1268,12 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="30"/>
       <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="29"/>
-    </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="U2" s="29"/>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>7</v>
@@ -1290,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1303,222 +1303,211 @@
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="30"/>
       <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="29"/>
-    </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="32"/>
+      <c r="U3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" s="3" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="33"/>
       <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="34"/>
-    </row>
-    <row r="5" spans="1:23" s="4" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="34"/>
+    </row>
+    <row r="5" spans="1:22" s="4" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="J5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="L5" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="N5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="Q5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="R5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" s="26" t="s">
-        <v>25</v>
-      </c>
+      <c r="S5" s="35"/>
       <c r="T5" s="35"/>
       <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="36"/>
-    </row>
-    <row r="6" spans="1:23" s="4" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="36"/>
+    </row>
+    <row r="6" spans="1:22" s="4" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="R6" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="19" t="s">
-        <v>41</v>
-      </c>
+      <c r="S6" s="35"/>
       <c r="T6" s="35"/>
       <c r="U6" s="35"/>
       <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-    </row>
-    <row r="7" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="22" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>65</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="O7" s="22" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="22" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="T7" s="37"/>
-    </row>
-    <row r="8" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+        <v>34</v>
+      </c>
+      <c r="S7" s="37"/>
+    </row>
+    <row r="8" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="22"/>
@@ -1526,21 +1515,20 @@
       <c r="E8" s="24"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
       <c r="O8" s="24"/>
       <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="37"/>
-    </row>
-    <row r="9" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q8" s="27"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="37"/>
+    </row>
+    <row r="9" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="22"/>
@@ -1548,21 +1536,20 @@
       <c r="E9" s="24"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="37"/>
-    </row>
-    <row r="10" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q9" s="27"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="37"/>
+    </row>
+    <row r="10" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="22"/>
@@ -1570,21 +1557,20 @@
       <c r="E10" s="24"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="37"/>
-    </row>
-    <row r="11" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q10" s="27"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="37"/>
+    </row>
+    <row r="11" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A11" s="22"/>
       <c r="B11" s="23"/>
       <c r="C11" s="22"/>
@@ -1592,21 +1578,20 @@
       <c r="E11" s="24"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
       <c r="N11" s="24"/>
       <c r="O11" s="24"/>
       <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="37"/>
-    </row>
-    <row r="12" spans="1:23" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q11" s="27"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="37"/>
+    </row>
+    <row r="12" spans="1:22" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A12" s="22"/>
       <c r="B12" s="23"/>
       <c r="C12" s="22"/>
@@ -1614,21 +1599,20 @@
       <c r="E12" s="24"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="37"/>
-    </row>
-    <row r="13" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q12" s="27"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="37"/>
+    </row>
+    <row r="13" spans="1:22" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A13" s="22"/>
       <c r="B13" s="23"/>
       <c r="C13" s="22"/>
@@ -1636,20 +1620,19 @@
       <c r="E13" s="24"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="24"/>
-    </row>
-    <row r="14" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q13" s="27"/>
+      <c r="R13" s="24"/>
+    </row>
+    <row r="14" spans="1:22" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="22"/>
@@ -1657,20 +1640,19 @@
       <c r="E14" s="24"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
       <c r="O14" s="24"/>
       <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="24"/>
-    </row>
-    <row r="15" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q14" s="27"/>
+      <c r="R14" s="24"/>
+    </row>
+    <row r="15" spans="1:22" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="22"/>
@@ -1678,20 +1660,19 @@
       <c r="E15" s="24"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="24"/>
-    </row>
-    <row r="16" spans="1:23" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q15" s="27"/>
+      <c r="R15" s="24"/>
+    </row>
+    <row r="16" spans="1:22" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="22"/>
@@ -1699,20 +1680,19 @@
       <c r="E16" s="24"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="H16" s="25"/>
       <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
       <c r="O16" s="24"/>
       <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="24"/>
-    </row>
-    <row r="17" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q16" s="27"/>
+      <c r="R16" s="24"/>
+    </row>
+    <row r="17" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A17" s="22"/>
       <c r="B17" s="23"/>
       <c r="C17" s="22"/>
@@ -1720,20 +1700,19 @@
       <c r="E17" s="24"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
       <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="24"/>
-    </row>
-    <row r="18" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q17" s="27"/>
+      <c r="R17" s="24"/>
+    </row>
+    <row r="18" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A18" s="22"/>
       <c r="B18" s="23"/>
       <c r="C18" s="22"/>
@@ -1741,20 +1720,19 @@
       <c r="E18" s="24"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="24"/>
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
       <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="24"/>
-    </row>
-    <row r="19" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q18" s="27"/>
+      <c r="R18" s="24"/>
+    </row>
+    <row r="19" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="22"/>
@@ -1762,20 +1740,19 @@
       <c r="E19" s="24"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
       <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="24"/>
-    </row>
-    <row r="20" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q19" s="27"/>
+      <c r="R19" s="24"/>
+    </row>
+    <row r="20" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A20" s="22"/>
       <c r="B20" s="23"/>
       <c r="C20" s="22"/>
@@ -1783,20 +1760,19 @@
       <c r="E20" s="24"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="24"/>
-    </row>
-    <row r="21" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q20" s="27"/>
+      <c r="R20" s="24"/>
+    </row>
+    <row r="21" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A21" s="22"/>
       <c r="B21" s="23"/>
       <c r="C21" s="22"/>
@@ -1804,20 +1780,19 @@
       <c r="E21" s="24"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
+      <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="24"/>
-    </row>
-    <row r="22" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q21" s="27"/>
+      <c r="R21" s="24"/>
+    </row>
+    <row r="22" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A22" s="22"/>
       <c r="B22" s="23"/>
       <c r="C22" s="22"/>
@@ -1825,20 +1800,19 @@
       <c r="E22" s="24"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
       <c r="O22" s="24"/>
       <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="24"/>
-    </row>
-    <row r="23" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q22" s="27"/>
+      <c r="R22" s="24"/>
+    </row>
+    <row r="23" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
       <c r="C23" s="22"/>
@@ -1846,20 +1820,19 @@
       <c r="E23" s="24"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="J23" s="24"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
       <c r="O23" s="24"/>
       <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="24"/>
-    </row>
-    <row r="24" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q23" s="27"/>
+      <c r="R23" s="24"/>
+    </row>
+    <row r="24" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A24" s="22"/>
       <c r="B24" s="23"/>
       <c r="C24" s="22"/>
@@ -1867,20 +1840,19 @@
       <c r="E24" s="24"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
+      <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
       <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="24"/>
-    </row>
-    <row r="25" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q24" s="27"/>
+      <c r="R24" s="24"/>
+    </row>
+    <row r="25" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A25" s="22"/>
       <c r="B25" s="23"/>
       <c r="C25" s="22"/>
@@ -1888,20 +1860,19 @@
       <c r="E25" s="24"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
+      <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="24"/>
-    </row>
-    <row r="26" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q25" s="27"/>
+      <c r="R25" s="24"/>
+    </row>
+    <row r="26" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A26" s="22"/>
       <c r="B26" s="23"/>
       <c r="C26" s="22"/>
@@ -1909,20 +1880,19 @@
       <c r="E26" s="24"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
       <c r="O26" s="24"/>
       <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="24"/>
-    </row>
-    <row r="27" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q26" s="27"/>
+      <c r="R26" s="24"/>
+    </row>
+    <row r="27" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A27" s="22"/>
       <c r="B27" s="23"/>
       <c r="C27" s="22"/>
@@ -1930,20 +1900,19 @@
       <c r="E27" s="24"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="J27" s="24"/>
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
       <c r="O27" s="24"/>
       <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="24"/>
-    </row>
-    <row r="28" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q27" s="27"/>
+      <c r="R27" s="24"/>
+    </row>
+    <row r="28" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A28" s="22"/>
       <c r="B28" s="23"/>
       <c r="C28" s="22"/>
@@ -1951,20 +1920,19 @@
       <c r="E28" s="24"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="J28" s="24"/>
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
       <c r="O28" s="24"/>
       <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="24"/>
-    </row>
-    <row r="29" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q28" s="27"/>
+      <c r="R28" s="24"/>
+    </row>
+    <row r="29" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A29" s="22"/>
       <c r="B29" s="23"/>
       <c r="C29" s="22"/>
@@ -1972,20 +1940,19 @@
       <c r="E29" s="24"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="H29" s="25"/>
       <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
       <c r="M29" s="24"/>
       <c r="N29" s="24"/>
       <c r="O29" s="24"/>
       <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="24"/>
-    </row>
-    <row r="30" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q29" s="27"/>
+      <c r="R29" s="24"/>
+    </row>
+    <row r="30" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A30" s="22"/>
       <c r="B30" s="23"/>
       <c r="C30" s="22"/>
@@ -1993,20 +1960,19 @@
       <c r="E30" s="24"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
+      <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="24"/>
       <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="24"/>
-    </row>
-    <row r="31" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q30" s="27"/>
+      <c r="R30" s="24"/>
+    </row>
+    <row r="31" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="22"/>
@@ -2014,20 +1980,19 @@
       <c r="E31" s="24"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
+      <c r="J31" s="24"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" s="24"/>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="24"/>
-    </row>
-    <row r="32" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q31" s="27"/>
+      <c r="R31" s="24"/>
+    </row>
+    <row r="32" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A32" s="22"/>
       <c r="B32" s="23"/>
       <c r="C32" s="22"/>
@@ -2035,20 +2000,19 @@
       <c r="E32" s="24"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="H32" s="25"/>
       <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
       <c r="O32" s="24"/>
       <c r="P32" s="24"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="27"/>
-      <c r="S32" s="24"/>
-    </row>
-    <row r="33" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q32" s="27"/>
+      <c r="R32" s="24"/>
+    </row>
+    <row r="33" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A33" s="22"/>
       <c r="B33" s="23"/>
       <c r="C33" s="22"/>
@@ -2056,20 +2020,19 @@
       <c r="E33" s="24"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
+      <c r="H33" s="25"/>
       <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
       <c r="N33" s="24"/>
       <c r="O33" s="24"/>
       <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="24"/>
-    </row>
-    <row r="34" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q33" s="27"/>
+      <c r="R33" s="24"/>
+    </row>
+    <row r="34" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A34" s="22"/>
       <c r="B34" s="23"/>
       <c r="C34" s="22"/>
@@ -2077,20 +2040,19 @@
       <c r="E34" s="24"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
+      <c r="H34" s="25"/>
       <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
+      <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" s="24"/>
       <c r="O34" s="24"/>
       <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="24"/>
-    </row>
-    <row r="35" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q34" s="27"/>
+      <c r="R34" s="24"/>
+    </row>
+    <row r="35" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A35" s="22"/>
       <c r="B35" s="23"/>
       <c r="C35" s="22"/>
@@ -2098,20 +2060,19 @@
       <c r="E35" s="24"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
+      <c r="H35" s="25"/>
       <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
+      <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" s="24"/>
       <c r="O35" s="24"/>
       <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="24"/>
-    </row>
-    <row r="36" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q35" s="27"/>
+      <c r="R35" s="24"/>
+    </row>
+    <row r="36" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A36" s="22"/>
       <c r="B36" s="23"/>
       <c r="C36" s="22"/>
@@ -2119,20 +2080,19 @@
       <c r="E36" s="24"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="H36" s="25"/>
       <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="J36" s="24"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
       <c r="M36" s="24"/>
       <c r="N36" s="24"/>
       <c r="O36" s="24"/>
       <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="24"/>
-    </row>
-    <row r="37" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q36" s="27"/>
+      <c r="R36" s="24"/>
+    </row>
+    <row r="37" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A37" s="22"/>
       <c r="B37" s="23"/>
       <c r="C37" s="22"/>
@@ -2140,20 +2100,19 @@
       <c r="E37" s="24"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="H37" s="25"/>
       <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
+      <c r="J37" s="24"/>
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24"/>
       <c r="O37" s="24"/>
       <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="27"/>
-      <c r="S37" s="24"/>
-    </row>
-    <row r="38" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q37" s="27"/>
+      <c r="R37" s="24"/>
+    </row>
+    <row r="38" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A38" s="22"/>
       <c r="B38" s="23"/>
       <c r="C38" s="22"/>
@@ -2161,20 +2120,19 @@
       <c r="E38" s="24"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
+      <c r="H38" s="25"/>
       <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
+      <c r="J38" s="24"/>
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
       <c r="M38" s="24"/>
       <c r="N38" s="24"/>
       <c r="O38" s="24"/>
       <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="24"/>
-    </row>
-    <row r="39" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q38" s="27"/>
+      <c r="R38" s="24"/>
+    </row>
+    <row r="39" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="22"/>
@@ -2182,20 +2140,19 @@
       <c r="E39" s="24"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
+      <c r="H39" s="25"/>
       <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="J39" s="24"/>
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
       <c r="M39" s="24"/>
       <c r="N39" s="24"/>
       <c r="O39" s="24"/>
       <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="24"/>
-    </row>
-    <row r="40" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q39" s="27"/>
+      <c r="R39" s="24"/>
+    </row>
+    <row r="40" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A40" s="22"/>
       <c r="B40" s="23"/>
       <c r="C40" s="22"/>
@@ -2203,20 +2160,19 @@
       <c r="E40" s="24"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
+      <c r="H40" s="25"/>
       <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
+      <c r="J40" s="24"/>
       <c r="K40" s="24"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24"/>
       <c r="O40" s="24"/>
       <c r="P40" s="24"/>
-      <c r="Q40" s="24"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="24"/>
-    </row>
-    <row r="41" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q40" s="27"/>
+      <c r="R40" s="24"/>
+    </row>
+    <row r="41" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A41" s="22"/>
       <c r="B41" s="23"/>
       <c r="C41" s="22"/>
@@ -2224,20 +2180,19 @@
       <c r="E41" s="24"/>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
+      <c r="J41" s="24"/>
       <c r="K41" s="24"/>
       <c r="L41" s="24"/>
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
       <c r="O41" s="24"/>
       <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="24"/>
-    </row>
-    <row r="42" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q41" s="27"/>
+      <c r="R41" s="24"/>
+    </row>
+    <row r="42" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A42" s="22"/>
       <c r="B42" s="23"/>
       <c r="C42" s="22"/>
@@ -2245,20 +2200,19 @@
       <c r="E42" s="24"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
+      <c r="H42" s="25"/>
       <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="J42" s="24"/>
       <c r="K42" s="24"/>
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
       <c r="N42" s="24"/>
       <c r="O42" s="24"/>
       <c r="P42" s="24"/>
-      <c r="Q42" s="24"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="24"/>
-    </row>
-    <row r="43" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q42" s="27"/>
+      <c r="R42" s="24"/>
+    </row>
+    <row r="43" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A43" s="22"/>
       <c r="B43" s="23"/>
       <c r="C43" s="22"/>
@@ -2266,20 +2220,19 @@
       <c r="E43" s="24"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
+      <c r="H43" s="25"/>
       <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="J43" s="24"/>
       <c r="K43" s="24"/>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
       <c r="O43" s="24"/>
       <c r="P43" s="24"/>
-      <c r="Q43" s="24"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="24"/>
-    </row>
-    <row r="44" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q43" s="27"/>
+      <c r="R43" s="24"/>
+    </row>
+    <row r="44" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A44" s="22"/>
       <c r="B44" s="23"/>
       <c r="C44" s="22"/>
@@ -2287,20 +2240,19 @@
       <c r="E44" s="24"/>
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
+      <c r="H44" s="25"/>
       <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
+      <c r="J44" s="24"/>
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
       <c r="N44" s="24"/>
       <c r="O44" s="24"/>
       <c r="P44" s="24"/>
-      <c r="Q44" s="24"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="24"/>
-    </row>
-    <row r="45" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q44" s="27"/>
+      <c r="R44" s="24"/>
+    </row>
+    <row r="45" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A45" s="22"/>
       <c r="B45" s="23"/>
       <c r="C45" s="22"/>
@@ -2308,20 +2260,19 @@
       <c r="E45" s="24"/>
       <c r="F45" s="22"/>
       <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
+      <c r="H45" s="25"/>
       <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="J45" s="24"/>
       <c r="K45" s="24"/>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
       <c r="N45" s="24"/>
       <c r="O45" s="24"/>
       <c r="P45" s="24"/>
-      <c r="Q45" s="24"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="24"/>
-    </row>
-    <row r="46" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q45" s="27"/>
+      <c r="R45" s="24"/>
+    </row>
+    <row r="46" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A46" s="22"/>
       <c r="B46" s="23"/>
       <c r="C46" s="22"/>
@@ -2329,20 +2280,19 @@
       <c r="E46" s="24"/>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
+      <c r="H46" s="25"/>
       <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="J46" s="24"/>
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
       <c r="N46" s="24"/>
       <c r="O46" s="24"/>
       <c r="P46" s="24"/>
-      <c r="Q46" s="24"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="24"/>
-    </row>
-    <row r="47" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q46" s="27"/>
+      <c r="R46" s="24"/>
+    </row>
+    <row r="47" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A47" s="22"/>
       <c r="B47" s="23"/>
       <c r="C47" s="22"/>
@@ -2350,20 +2300,19 @@
       <c r="E47" s="24"/>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
+      <c r="H47" s="25"/>
       <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
+      <c r="J47" s="24"/>
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
       <c r="N47" s="24"/>
       <c r="O47" s="24"/>
       <c r="P47" s="24"/>
-      <c r="Q47" s="24"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="24"/>
-    </row>
-    <row r="48" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q47" s="27"/>
+      <c r="R47" s="24"/>
+    </row>
+    <row r="48" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A48" s="22"/>
       <c r="B48" s="23"/>
       <c r="C48" s="22"/>
@@ -2371,20 +2320,19 @@
       <c r="E48" s="24"/>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
+      <c r="H48" s="25"/>
       <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
+      <c r="J48" s="24"/>
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
       <c r="M48" s="24"/>
       <c r="N48" s="24"/>
       <c r="O48" s="24"/>
       <c r="P48" s="24"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="27"/>
-      <c r="S48" s="24"/>
-    </row>
-    <row r="49" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q48" s="27"/>
+      <c r="R48" s="24"/>
+    </row>
+    <row r="49" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A49" s="22"/>
       <c r="B49" s="23"/>
       <c r="C49" s="22"/>
@@ -2392,20 +2340,19 @@
       <c r="E49" s="24"/>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
+      <c r="H49" s="25"/>
       <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
+      <c r="J49" s="24"/>
       <c r="K49" s="24"/>
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" s="24"/>
       <c r="O49" s="24"/>
       <c r="P49" s="24"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="27"/>
-      <c r="S49" s="24"/>
-    </row>
-    <row r="50" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q49" s="27"/>
+      <c r="R49" s="24"/>
+    </row>
+    <row r="50" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A50" s="22"/>
       <c r="B50" s="23"/>
       <c r="C50" s="22"/>
@@ -2413,20 +2360,19 @@
       <c r="E50" s="24"/>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
+      <c r="H50" s="25"/>
       <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
+      <c r="J50" s="24"/>
       <c r="K50" s="24"/>
       <c r="L50" s="24"/>
       <c r="M50" s="24"/>
       <c r="N50" s="24"/>
       <c r="O50" s="24"/>
       <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="27"/>
-      <c r="S50" s="24"/>
-    </row>
-    <row r="51" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q50" s="27"/>
+      <c r="R50" s="24"/>
+    </row>
+    <row r="51" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A51" s="22"/>
       <c r="B51" s="23"/>
       <c r="C51" s="22"/>
@@ -2434,20 +2380,19 @@
       <c r="E51" s="24"/>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
+      <c r="H51" s="25"/>
       <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
+      <c r="J51" s="24"/>
       <c r="K51" s="24"/>
       <c r="L51" s="24"/>
       <c r="M51" s="24"/>
       <c r="N51" s="24"/>
       <c r="O51" s="24"/>
       <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="24"/>
-    </row>
-    <row r="52" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q51" s="27"/>
+      <c r="R51" s="24"/>
+    </row>
+    <row r="52" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A52" s="22"/>
       <c r="B52" s="23"/>
       <c r="C52" s="22"/>
@@ -2455,20 +2400,19 @@
       <c r="E52" s="24"/>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
+      <c r="H52" s="25"/>
       <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
+      <c r="J52" s="24"/>
       <c r="K52" s="24"/>
       <c r="L52" s="24"/>
       <c r="M52" s="24"/>
       <c r="N52" s="24"/>
       <c r="O52" s="24"/>
       <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="27"/>
-      <c r="S52" s="24"/>
-    </row>
-    <row r="53" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q52" s="27"/>
+      <c r="R52" s="24"/>
+    </row>
+    <row r="53" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A53" s="22"/>
       <c r="B53" s="23"/>
       <c r="C53" s="22"/>
@@ -2476,20 +2420,19 @@
       <c r="E53" s="24"/>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
+      <c r="H53" s="25"/>
       <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
+      <c r="J53" s="24"/>
       <c r="K53" s="24"/>
       <c r="L53" s="24"/>
       <c r="M53" s="24"/>
       <c r="N53" s="24"/>
       <c r="O53" s="24"/>
       <c r="P53" s="24"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="27"/>
-      <c r="S53" s="24"/>
-    </row>
-    <row r="54" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q53" s="27"/>
+      <c r="R53" s="24"/>
+    </row>
+    <row r="54" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A54" s="22"/>
       <c r="B54" s="23"/>
       <c r="C54" s="22"/>
@@ -2497,20 +2440,19 @@
       <c r="E54" s="24"/>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
+      <c r="H54" s="25"/>
       <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
+      <c r="J54" s="24"/>
       <c r="K54" s="24"/>
       <c r="L54" s="24"/>
       <c r="M54" s="24"/>
       <c r="N54" s="24"/>
       <c r="O54" s="24"/>
       <c r="P54" s="24"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="24"/>
-    </row>
-    <row r="55" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q54" s="27"/>
+      <c r="R54" s="24"/>
+    </row>
+    <row r="55" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A55" s="22"/>
       <c r="B55" s="23"/>
       <c r="C55" s="22"/>
@@ -2518,20 +2460,19 @@
       <c r="E55" s="24"/>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
+      <c r="H55" s="25"/>
       <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
+      <c r="J55" s="24"/>
       <c r="K55" s="24"/>
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
       <c r="N55" s="24"/>
       <c r="O55" s="24"/>
       <c r="P55" s="24"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="27"/>
-      <c r="S55" s="24"/>
-    </row>
-    <row r="56" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q55" s="27"/>
+      <c r="R55" s="24"/>
+    </row>
+    <row r="56" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A56" s="22"/>
       <c r="B56" s="23"/>
       <c r="C56" s="22"/>
@@ -2539,20 +2480,19 @@
       <c r="E56" s="24"/>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
+      <c r="H56" s="25"/>
       <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
+      <c r="J56" s="24"/>
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
       <c r="M56" s="24"/>
       <c r="N56" s="24"/>
       <c r="O56" s="24"/>
       <c r="P56" s="24"/>
-      <c r="Q56" s="24"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="24"/>
-    </row>
-    <row r="57" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q56" s="27"/>
+      <c r="R56" s="24"/>
+    </row>
+    <row r="57" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A57" s="22"/>
       <c r="B57" s="23"/>
       <c r="C57" s="22"/>
@@ -2560,20 +2500,19 @@
       <c r="E57" s="24"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
+      <c r="H57" s="25"/>
       <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
+      <c r="J57" s="24"/>
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
       <c r="N57" s="24"/>
       <c r="O57" s="24"/>
       <c r="P57" s="24"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="27"/>
-      <c r="S57" s="24"/>
-    </row>
-    <row r="58" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q57" s="27"/>
+      <c r="R57" s="24"/>
+    </row>
+    <row r="58" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A58" s="22"/>
       <c r="B58" s="23"/>
       <c r="C58" s="22"/>
@@ -2581,20 +2520,19 @@
       <c r="E58" s="24"/>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
+      <c r="H58" s="25"/>
       <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
+      <c r="J58" s="24"/>
       <c r="K58" s="24"/>
       <c r="L58" s="24"/>
       <c r="M58" s="24"/>
       <c r="N58" s="24"/>
       <c r="O58" s="24"/>
       <c r="P58" s="24"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="27"/>
-      <c r="S58" s="24"/>
-    </row>
-    <row r="59" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q58" s="27"/>
+      <c r="R58" s="24"/>
+    </row>
+    <row r="59" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A59" s="22"/>
       <c r="B59" s="23"/>
       <c r="C59" s="22"/>
@@ -2602,20 +2540,19 @@
       <c r="E59" s="24"/>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
+      <c r="H59" s="25"/>
       <c r="I59" s="25"/>
-      <c r="J59" s="25"/>
+      <c r="J59" s="24"/>
       <c r="K59" s="24"/>
       <c r="L59" s="24"/>
       <c r="M59" s="24"/>
       <c r="N59" s="24"/>
       <c r="O59" s="24"/>
       <c r="P59" s="24"/>
-      <c r="Q59" s="24"/>
-      <c r="R59" s="27"/>
-      <c r="S59" s="24"/>
-    </row>
-    <row r="60" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q59" s="27"/>
+      <c r="R59" s="24"/>
+    </row>
+    <row r="60" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A60" s="22"/>
       <c r="B60" s="23"/>
       <c r="C60" s="22"/>
@@ -2623,20 +2560,19 @@
       <c r="E60" s="24"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
+      <c r="H60" s="25"/>
       <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
+      <c r="J60" s="24"/>
       <c r="K60" s="24"/>
       <c r="L60" s="24"/>
       <c r="M60" s="24"/>
       <c r="N60" s="24"/>
       <c r="O60" s="24"/>
       <c r="P60" s="24"/>
-      <c r="Q60" s="24"/>
-      <c r="R60" s="27"/>
-      <c r="S60" s="24"/>
-    </row>
-    <row r="61" spans="1:19" ht="14.5" x14ac:dyDescent="0.4">
+      <c r="Q60" s="27"/>
+      <c r="R60" s="24"/>
+    </row>
+    <row r="61" spans="1:18" ht="14.5" x14ac:dyDescent="0.4">
       <c r="A61" s="22"/>
       <c r="B61" s="23"/>
       <c r="C61" s="22"/>
@@ -2644,23 +2580,22 @@
       <c r="E61" s="24"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
+      <c r="H61" s="25"/>
       <c r="I61" s="25"/>
-      <c r="J61" s="25"/>
+      <c r="J61" s="24"/>
       <c r="K61" s="24"/>
       <c r="L61" s="24"/>
       <c r="M61" s="24"/>
       <c r="N61" s="24"/>
       <c r="O61" s="24"/>
       <c r="P61" s="24"/>
-      <c r="Q61" s="24"/>
-      <c r="R61" s="27"/>
-      <c r="S61" s="24"/>
+      <c r="Q61" s="27"/>
+      <c r="R61" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A4:R4"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>